<commit_message>
InApkStringTable, StringTable 이 있는 엑셀 커밋
</commit_message>
<xml_diff>
--- a/Excel/String.xlsx
+++ b/Excel/String.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D1BFC9A-2357-4C89-994F-697255E8DFFE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E299F04C-D4BA-4D6C-A1EB-B4D4FDAD0241}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TitleStringTable" sheetId="2" r:id="rId1"/>
+    <sheet name="InApkStringTable" sheetId="2" r:id="rId1"/>
     <sheet name="StringTable" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>확인</t>
   </si>
@@ -58,9 +58,6 @@
 &lt;color=cyan&gt;와이파이&lt;/color&gt;를 사용해서 다운로드 받으시길 권장합니다.</t>
   </si>
   <si>
-    <t>New Patch!</t>
-  </si>
-  <si>
     <t>서버와의 접속이 원활하지 않습니다.
 프로그램을 재시작합니다.</t>
   </si>
@@ -178,6 +175,90 @@
   </si>
   <si>
     <t>Use Repair Kit Lv. {0}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hearts exploding!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Patch!
+Recommended to download with &lt;color=cyan&gt;WIFI&lt;/color&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bad connection
+Restarting the app</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUI_PossibleAfterTraining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>훈련 챕터 클리어 후 진행 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Possible to play after the training chapter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUI_Shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상점</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameUI_UnderConstruction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>개발 중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Under Construction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemUI_Mainternance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버 점검 중입니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We're on a mainternance</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We will be performing scheduled maintenance on Tuesday, May 29th. Maintenance will begin at 3:00 AM PDT and conclude at approximately 11:00 AM PDT. During this time, servers and many web services will be unavailable.
+Thank you for your patience.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SystemUI_MainternanceDetail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5월 29일 화요일 오전 3시부터 대략 11시까지 정기 점검 예정입니다. 이 동안 서버 및 웹 서비스 등을 사용하실 수 없습니다.
+감사합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal &lt;color=#FFFF00&gt;{0}%,{1}%,{2}%,{3}%&lt;/color&gt; and then the enemy drops a heart if killed. If not, stunned.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Deal &lt;color=#FFFF00&gt;{0}%&lt;/color&gt; and then the enemy drops a heart if killed. If not, stunned.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,201 +650,266 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="67.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="33" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.875" customWidth="1"/>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
     <col min="2" max="2" width="97.25" customWidth="1"/>
     <col min="3" max="3" width="78.375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="29.625" customWidth="1"/>
+    <col min="2" max="2" width="97.25" customWidth="1"/>
+    <col min="3" max="3" width="78.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="33" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POWER 및 Chpater 텍스트 조정
</commit_message>
<xml_diff>
--- a/Excel/String.xlsx
+++ b/Excel/String.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD573614-12C6-4173-BB3C-AD6920CF9C8A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F8E861-98F0-47B6-AA04-AE630D31A521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2022,14 +2022,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>챕터 {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Chapter {0}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>GameUI_RomanNumber1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2279,10 +2271,6 @@
   </si>
   <si>
     <t>GameUI_Power</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>POWER {0}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2608,6 +2596,18 @@
   </si>
   <si>
     <t>GameUI_NowPlayingCharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>챕터</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Chapter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;color=#E0E0E0&gt;POWER&lt;/color&gt; &lt;size=17&gt;{0}&lt;/size&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3014,9 +3014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3137,332 +3135,332 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C11" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C12" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C13" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C14" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C15" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C16" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C17" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C18" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C19" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C20" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B21" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="C21" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B22" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="C22" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C23" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B24" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="C24" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B25" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C25" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B26" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C26" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B27" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C27" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="C28" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B29" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C29" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C30" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B31" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C31" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B32" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C32" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B33" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C33" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B34" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="C34" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B35" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C35" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B36" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="C36" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B37" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C37" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B38" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="C38" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B39" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C39" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B40" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C40" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -3511,90 +3509,90 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -3745,7 +3743,7 @@
         <v>358</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" ref="C66" si="0">"In progress of translating…("&amp;ROW()&amp;")"</f>
@@ -3768,76 +3766,76 @@
         <v>428</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>429</v>
+        <v>599</v>
       </c>
       <c r="C68" t="s">
-        <v>430</v>
+        <v>600</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>501</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="C69" t="s">
         <v>503</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>504</v>
-      </c>
-      <c r="C69" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="C70" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>509</v>
+        <v>601</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>509</v>
+        <v>601</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
@@ -5437,10 +5435,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B209" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="C209" t="str">
         <f t="shared" si="2"/>
@@ -5449,10 +5447,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B210" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C210" t="str">
         <f t="shared" si="2"/>
@@ -5461,10 +5459,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="B211" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C211" t="str">
         <f t="shared" si="2"/>
@@ -5473,10 +5471,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B212" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C212" t="str">
         <f t="shared" si="2"/>
@@ -5485,10 +5483,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B213" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C213" t="str">
         <f t="shared" si="2"/>
@@ -5497,10 +5495,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="B214" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C214" t="str">
         <f t="shared" si="2"/>
@@ -5509,10 +5507,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B215" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C215" t="str">
         <f t="shared" si="2"/>
@@ -5521,10 +5519,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B216" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="C216" t="str">
         <f t="shared" si="2"/>
@@ -5608,7 +5606,7 @@
         <v>320</v>
       </c>
       <c r="B223" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C223" t="str">
         <f t="shared" si="2"/>
@@ -5776,7 +5774,7 @@
         <v>334</v>
       </c>
       <c r="B237" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="C237" t="str">
         <f t="shared" si="2"/>
@@ -5785,10 +5783,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B238" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="C238" t="str">
         <f t="shared" si="2"/>
@@ -5797,10 +5795,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B239" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C239" t="str">
         <f t="shared" si="2"/>
@@ -5809,10 +5807,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="B240" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="C240" t="str">
         <f t="shared" si="2"/>
@@ -5821,10 +5819,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B241" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C241" t="str">
         <f t="shared" si="2"/>
@@ -5833,10 +5831,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B242" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="C242" t="str">
         <f t="shared" si="2"/>
@@ -5845,10 +5843,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="B243" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="C243" t="str">
         <f t="shared" si="2"/>
@@ -5857,10 +5855,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B244" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="C244" t="str">
         <f t="shared" si="2"/>
@@ -5869,10 +5867,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="B245" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="C245" t="str">
         <f t="shared" si="2"/>
@@ -5881,21 +5879,21 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B246" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C246" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="66" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C247" t="str">
         <f t="shared" si="2"/>
@@ -5904,21 +5902,21 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="B248" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C248" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="249" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C249" t="str">
         <f t="shared" si="2"/>
@@ -5927,21 +5925,21 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B250" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C250" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="251" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="C251" t="str">
         <f t="shared" si="2"/>
@@ -5950,21 +5948,21 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B252" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C252" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="253" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B253" s="1" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C253" t="str">
         <f t="shared" si="2"/>
@@ -5973,10 +5971,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B254" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C254" t="str">
         <f t="shared" si="2"/>
@@ -6000,7 +5998,7 @@
         <v>381</v>
       </c>
       <c r="B256" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C256" t="str">
         <f t="shared" si="2"/>
@@ -6012,7 +6010,7 @@
         <v>382</v>
       </c>
       <c r="B257" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C257" t="str">
         <f t="shared" si="2"/>
@@ -6024,7 +6022,7 @@
         <v>380</v>
       </c>
       <c r="B258" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C258" t="str">
         <f t="shared" si="2"/>
@@ -6036,7 +6034,7 @@
         <v>384</v>
       </c>
       <c r="B259" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C259" t="str">
         <f t="shared" si="2"/>
@@ -6048,7 +6046,7 @@
         <v>385</v>
       </c>
       <c r="B260" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C260" t="str">
         <f t="shared" si="2"/>
@@ -6060,7 +6058,7 @@
         <v>383</v>
       </c>
       <c r="B261" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C261" t="str">
         <f t="shared" si="2"/>

</xml_diff>